<commit_message>
Added row-based DF appending notebook.
</commit_message>
<xml_diff>
--- a/Top.xlsx
+++ b/Top.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Teaching\Undergraduate Courses\Network Science (CZ4071)\2021\Assignments\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthur\git\ns-project-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E288F994-A2C0-49F0-BCDE-BB19856B9797}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C0FFB4-C96E-4217-B6FC-A1FAAC704450}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10980" xr2:uid="{DAE53E0A-6A05-4D41-9D1F-4972FBFE7488}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11746" xr2:uid="{DAE53E0A-6A05-4D41-9D1F-4972FBFE7488}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Area</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>ACM RECOMB</t>
+  </si>
+  <si>
+    <t>DBLP Code</t>
   </si>
 </sst>
 </file>
@@ -502,19 +505,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54268E5D-2F4B-46C0-BD24-65ED2E7F2031}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="29.36328125" customWidth="1"/>
-    <col min="2" max="2" width="14.58984375" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -524,8 +527,11 @@
       <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -533,7 +539,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -541,7 +547,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -549,7 +555,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -557,7 +563,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -568,7 +574,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -576,7 +582,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -584,7 +590,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -592,7 +598,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -603,7 +609,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -611,7 +617,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -619,7 +625,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -627,7 +633,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -635,7 +641,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>23</v>
       </c>

</xml_diff>